<commit_message>
Switched to use the DOSE_RECEIVED indication type
</commit_message>
<xml_diff>
--- a/schedules/MeningBexsero.xlsx
+++ b/schedules/MeningBexsero.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="45" windowWidth="19335" windowHeight="18585" tabRatio="396"/>
+    <workbookView xWindow="17340" yWindow="45" windowWidth="19335" windowHeight="18240" tabRatio="396"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
@@ -170,10 +170,10 @@
     <t>19 years</t>
   </si>
   <si>
-    <t>BIRTH</t>
-  </si>
-  <si>
     <t>MeningBexsero</t>
+  </si>
+  <si>
+    <t>DOSERECEIVED</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -540,7 +540,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -835,7 +835,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -877,7 +877,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -894,7 +894,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -905,7 +905,7 @@
   <dimension ref="B1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -932,7 +932,7 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" s="25" t="s">
         <v>1</v>
@@ -1074,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="2:9">
@@ -1399,7 +1399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -1421,7 +1423,7 @@
     <row r="3" spans="1:1">
       <c r="A3" s="21" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B22&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C22&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D22&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E21&amp;CHAR(34)&amp;"&gt;"</f>
-        <v xml:space="preserve">  &lt;schedule scheduleName="B1" dose="1" indication="BIRTH" label="1st"&gt;</v>
+        <v xml:space="preserve">  &lt;schedule scheduleName="B1" dose="1" indication="DOSERECEIVED" label="1st"&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:1">

</xml_diff>